<commit_message>
Add mimic 10 to processing
</commit_message>
<xml_diff>
--- a/data/tumor-size/AOT00041318-mimic01/AOT00041318_size-measurements.xlsx
+++ b/data/tumor-size/AOT00041318-mimic01/AOT00041318_size-measurements.xlsx
@@ -1,58 +1,78 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25412"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wil407\Box Sync\mimic\data\AOT00041318\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wil407\Box Sync\mimic\data\AOT00041318-mimic01\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4483177F-5C06-46F4-8D3B-31DE0159F2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="44">
+  <si>
+    <t>date</t>
+  </si>
   <si>
     <t>tail.number</t>
   </si>
   <si>
+    <t>treatment</t>
+  </si>
+  <si>
     <t>microbiome.sample</t>
   </si>
   <si>
-    <t>treatment</t>
-  </si>
-  <si>
-    <t>date</t>
+    <t>weight.(g)</t>
+  </si>
+  <si>
+    <t>tumor.size.(mm)</t>
+  </si>
+  <si>
+    <t>tumor.length.(mm)</t>
+  </si>
+  <si>
+    <t>tumor.width.(mm)</t>
+  </si>
+  <si>
+    <t>Anti-PD-1</t>
+  </si>
+  <si>
+    <t>HONC-60-55.v3</t>
   </si>
   <si>
     <t>IgG</t>
   </si>
   <si>
-    <t>Anti-PD-1</t>
-  </si>
-  <si>
-    <t>HONC-60-55.v3</t>
-  </si>
-  <si>
     <t>HONC-60-55.v4</t>
   </si>
   <si>
-    <t>weight.(g)</t>
-  </si>
-  <si>
     <t>5.8 x 3.8</t>
   </si>
   <si>
@@ -80,6 +100,30 @@
     <t>5.4 x 2.8</t>
   </si>
   <si>
+    <t>11.0 x 7.0</t>
+  </si>
+  <si>
+    <t>10 x 8.5</t>
+  </si>
+  <si>
+    <t>12 x 6.0</t>
+  </si>
+  <si>
+    <t>8.5 x 6.9</t>
+  </si>
+  <si>
+    <t>5.5 x 4.5</t>
+  </si>
+  <si>
+    <t>7.9 x 4.9</t>
+  </si>
+  <si>
+    <t>5.7 x 3.3</t>
+  </si>
+  <si>
+    <t>7.0 x 5.6 &amp; 5.2 x 3.0</t>
+  </si>
+  <si>
     <t>9.2 x 6.5</t>
   </si>
   <si>
@@ -113,6 +157,9 @@
     <t>15.7 x 14.1</t>
   </si>
   <si>
+    <t>11.5 x 11.5 &amp; 11.5 x 10.8</t>
+  </si>
+  <si>
     <t>12.8 x 8.3</t>
   </si>
   <si>
@@ -120,52 +167,16 @@
   </si>
   <si>
     <t>5.4 x 4.1</t>
-  </si>
-  <si>
-    <t>tumor.size.(mm)</t>
-  </si>
-  <si>
-    <t>11.0 x 7.0</t>
-  </si>
-  <si>
-    <t>10 x 8.5</t>
-  </si>
-  <si>
-    <t>12 x 6.0</t>
-  </si>
-  <si>
-    <t>8.5 x 6.9</t>
-  </si>
-  <si>
-    <t>5.5 x 4.5</t>
-  </si>
-  <si>
-    <t>7.9 x 4.9</t>
-  </si>
-  <si>
-    <t>5.7 x 3.3</t>
-  </si>
-  <si>
-    <t>7.0 x 5.6 &amp; 5.2 x 3.0</t>
-  </si>
-  <si>
-    <t>11.5 x 11.5 &amp; 11.5 x 10.8</t>
-  </si>
-  <si>
-    <t>tumor.length.(mm)</t>
-  </si>
-  <si>
-    <t>tumor.width.(mm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,11 +211,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,14 +528,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.875" customWidth="1"/>
     <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
@@ -537,33 +547,33 @@
     <col min="8" max="8" width="16.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>44341</v>
       </c>
@@ -571,10 +581,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>25.2</v>
@@ -586,7 +596,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>44341</v>
       </c>
@@ -594,10 +604,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>27</v>
@@ -608,17 +618,8 @@
       <c r="H3">
         <v>3.3</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>44341</v>
       </c>
@@ -626,10 +627,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>26.3</v>
@@ -641,7 +642,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>44341</v>
       </c>
@@ -649,10 +650,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>23</v>
@@ -664,7 +665,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>44341</v>
       </c>
@@ -672,10 +673,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -687,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>44341</v>
       </c>
@@ -695,10 +696,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>23.3</v>
@@ -710,7 +711,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>44341</v>
       </c>
@@ -718,10 +719,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>25.9</v>
@@ -733,7 +734,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>44341</v>
       </c>
@@ -741,10 +742,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <v>26.2</v>
@@ -756,7 +757,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>44341</v>
       </c>
@@ -764,10 +765,10 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>26</v>
@@ -779,7 +780,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>44341</v>
       </c>
@@ -787,10 +788,10 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E11">
         <v>26</v>
@@ -802,7 +803,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>44343</v>
       </c>
@@ -810,25 +811,25 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
         <v>25.3</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>5.8</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12">
         <v>3.8</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>44343</v>
       </c>
@@ -836,16 +837,16 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2">
         <v>26.6</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G13">
         <v>7.4</v>
@@ -854,7 +855,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>44343</v>
       </c>
@@ -862,16 +863,16 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2">
         <v>26.8</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G14">
         <v>3.3</v>
@@ -880,7 +881,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>44343</v>
       </c>
@@ -888,16 +889,16 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E15" s="2">
         <v>23.4</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G15">
         <v>5.0999999999999996</v>
@@ -906,7 +907,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>44343</v>
       </c>
@@ -914,16 +915,16 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E16" s="2">
         <v>25.2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>44343</v>
       </c>
@@ -931,16 +932,16 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E17" s="2">
         <v>23.3</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G17">
         <v>3.3</v>
@@ -949,7 +950,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>44343</v>
       </c>
@@ -957,16 +958,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E18" s="2">
         <v>26.2</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G18">
         <v>4.2</v>
@@ -975,7 +976,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>44343</v>
       </c>
@@ -983,16 +984,16 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E19" s="2">
         <v>25.5</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G19">
         <v>5.4</v>
@@ -1001,7 +1002,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>44343</v>
       </c>
@@ -1009,16 +1010,16 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E20" s="2">
         <v>25.9</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G20">
         <v>4.8</v>
@@ -1027,7 +1028,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>44343</v>
       </c>
@@ -1035,16 +1036,16 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E21" s="2">
         <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G21">
         <v>5.4</v>
@@ -1053,7 +1054,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>44347</v>
       </c>
@@ -1061,16 +1062,16 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E22" s="2">
         <v>25.9</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>44347</v>
       </c>
@@ -1078,16 +1079,16 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E23" s="2">
         <v>24.9</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G23">
         <v>11</v>
@@ -1096,7 +1097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>44347</v>
       </c>
@@ -1104,16 +1105,16 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E24" s="2">
         <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G24">
         <v>10</v>
@@ -1122,7 +1123,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>44347</v>
       </c>
@@ -1130,16 +1131,16 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E25" s="2">
         <v>25.2</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="G25">
         <v>12</v>
@@ -1148,7 +1149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>44347</v>
       </c>
@@ -1156,16 +1157,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E26" s="2">
         <v>25.9</v>
       </c>
       <c r="F26" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G26">
         <v>8.5</v>
@@ -1174,7 +1175,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <v>44347</v>
       </c>
@@ -1182,16 +1183,16 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E27" s="2">
         <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G27">
         <v>5.5</v>
@@ -1200,7 +1201,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>44347</v>
       </c>
@@ -1208,16 +1209,16 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E28" s="2">
         <v>26.5</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G28">
         <v>7.9</v>
@@ -1226,7 +1227,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>44347</v>
       </c>
@@ -1234,16 +1235,16 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E29" s="2">
         <v>23.8</v>
       </c>
       <c r="F29" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="G29">
         <v>5.7</v>
@@ -1252,7 +1253,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <v>44347</v>
       </c>
@@ -1260,16 +1261,16 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E30" s="2">
         <v>26.1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>44347</v>
       </c>
@@ -1277,16 +1278,16 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E31" s="2">
         <v>26</v>
       </c>
       <c r="F31" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="G31">
         <v>7</v>
@@ -1295,7 +1296,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
         <v>44347</v>
       </c>
@@ -1303,16 +1304,16 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E32" s="2">
         <v>26</v>
       </c>
       <c r="F32" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="G32">
         <v>5.2</v>
@@ -1321,7 +1322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>44350</v>
       </c>
@@ -1329,10 +1330,10 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E33" s="2"/>
       <c r="G33">
@@ -1342,7 +1343,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>44350</v>
       </c>
@@ -1350,10 +1351,10 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G34">
         <v>2.8</v>
@@ -1362,7 +1363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>44350</v>
       </c>
@@ -1370,10 +1371,10 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G35">
         <v>5.3</v>
@@ -1382,7 +1383,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>44350</v>
       </c>
@@ -1390,10 +1391,10 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G36">
         <v>11.3</v>
@@ -1402,7 +1403,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>44350</v>
       </c>
@@ -1410,10 +1411,10 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -1422,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>44350</v>
       </c>
@@ -1430,10 +1431,10 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G38">
         <v>7.7</v>
@@ -1442,7 +1443,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>44350</v>
       </c>
@@ -1450,10 +1451,10 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G39">
         <v>3.8</v>
@@ -1462,7 +1463,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="1">
         <v>44350</v>
       </c>
@@ -1470,10 +1471,10 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G40">
         <v>5.7</v>
@@ -1482,7 +1483,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="1">
         <v>44350</v>
       </c>
@@ -1490,10 +1491,10 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G41">
         <v>9.6</v>
@@ -1502,7 +1503,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>44350</v>
       </c>
@@ -1510,10 +1511,10 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G42">
         <v>13.8</v>
@@ -1522,7 +1523,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="1">
         <v>44353</v>
       </c>
@@ -1530,16 +1531,16 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E43" s="2">
         <v>26</v>
       </c>
       <c r="F43" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="G43">
         <v>9.1999999999999993</v>
@@ -1548,7 +1549,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="1">
         <v>44353</v>
       </c>
@@ -1556,16 +1557,16 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E44" s="2">
         <v>24.68</v>
       </c>
       <c r="F44" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G44">
         <v>13.8</v>
@@ -1574,7 +1575,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="1">
         <v>44353</v>
       </c>
@@ -1582,16 +1583,16 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E45" s="2">
         <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G45">
         <v>18.100000000000001</v>
@@ -1600,7 +1601,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="1">
         <v>44353</v>
       </c>
@@ -1608,16 +1609,16 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E46" s="2">
         <v>25.3</v>
       </c>
       <c r="F46" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G46">
         <v>19</v>
@@ -1626,7 +1627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>44353</v>
       </c>
@@ -1634,16 +1635,16 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E47" s="2">
         <v>26.5</v>
       </c>
       <c r="F47" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="G47">
         <v>9.5</v>
@@ -1652,7 +1653,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="1">
         <v>44353</v>
       </c>
@@ -1660,16 +1661,16 @@
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E48" s="2">
         <v>27.1</v>
       </c>
       <c r="F48" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G48">
         <v>2</v>
@@ -1678,7 +1679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="1">
         <v>44353</v>
       </c>
@@ -1686,16 +1687,16 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E49" s="2">
         <v>26.1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="1">
         <v>44353</v>
       </c>
@@ -1703,16 +1704,16 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E50" s="2">
         <v>23.9</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="1">
         <v>44353</v>
       </c>
@@ -1720,16 +1721,16 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E51" s="2">
         <v>26.3</v>
       </c>
       <c r="F51" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>7.1</v>
@@ -1738,7 +1739,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="1">
         <v>44353</v>
       </c>
@@ -1746,16 +1747,16 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E52" s="2">
         <v>26</v>
       </c>
       <c r="F52" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="G52">
         <v>6.5</v>
@@ -1764,7 +1765,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="1">
         <v>44356</v>
       </c>
@@ -1772,16 +1773,16 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E53" s="2">
         <v>25.8</v>
       </c>
       <c r="F53" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G53">
         <v>10</v>
@@ -1790,7 +1791,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="1">
         <v>44356</v>
       </c>
@@ -1798,16 +1799,16 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E54" s="2">
         <v>24.6</v>
       </c>
       <c r="F54" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="G54">
         <v>15.2</v>
@@ -1816,7 +1817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="1">
         <v>44356</v>
       </c>
@@ -1824,16 +1825,16 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E55" s="2">
         <v>26.7</v>
       </c>
       <c r="F55" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G55">
         <v>15.7</v>
@@ -1842,7 +1843,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="1">
         <v>44356</v>
       </c>
@@ -1850,16 +1851,16 @@
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E56" s="2">
         <v>25.5</v>
       </c>
       <c r="F56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G56">
         <v>11.5</v>
@@ -1868,158 +1869,132 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="1">
         <v>44356</v>
       </c>
       <c r="B57">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E57" s="2">
-        <v>25.5</v>
+        <v>26.4</v>
       </c>
       <c r="F57" t="s">
         <v>41</v>
       </c>
       <c r="G57">
-        <v>11.5</v>
+        <v>12.8</v>
       </c>
       <c r="H57">
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="1">
         <v>44356</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E58" s="2">
-        <v>26.4</v>
-      </c>
-      <c r="F58" t="s">
-        <v>29</v>
-      </c>
-      <c r="G58">
-        <v>12.8</v>
-      </c>
-      <c r="H58">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="1">
         <v>44356</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E59" s="2">
-        <v>26.3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="1">
         <v>44356</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E60" s="2">
-        <v>25.7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="1">
         <v>44356</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E61" s="2">
-        <v>23.9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26.3</v>
+      </c>
+      <c r="F61" t="s">
+        <v>42</v>
+      </c>
+      <c r="G61">
+        <v>7.6</v>
+      </c>
+      <c r="H61">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="1">
         <v>44356</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E62" s="2">
-        <v>26.3</v>
+        <v>25.8</v>
       </c>
       <c r="F62" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G62">
-        <v>7.6</v>
+        <v>5.4</v>
       </c>
       <c r="H62">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>44356</v>
-      </c>
-      <c r="B63">
-        <v>3</v>
-      </c>
-      <c r="C63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" s="2">
-        <v>25.8</v>
-      </c>
-      <c r="F63" t="s">
-        <v>31</v>
-      </c>
-      <c r="G63">
-        <v>5.4</v>
-      </c>
-      <c r="H63">
         <v>4.0999999999999996</v>
       </c>
     </row>

</xml_diff>